<commit_message>
Edited C7 data and ran lm to figure out the different intercept between C7 data and chlor-a extractions
</commit_message>
<xml_diff>
--- a/gl4.buoy.RBRTemp.xlsx
+++ b/gl4.buoy.RBRTemp.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellyloria/Documents/Niwot LTER 2017-2019/GL4 Sensor/Buoy Data/Buoy_QAQC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C495929-5583-5246-A221-28E8B432E999}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{1CCC06D4-7BE2-2E43-ADAD-A5705792E327}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="460" windowWidth="20760" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8040" yWindow="460" windowWidth="20760" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="gl4_buyRBRTemp.meta" sheetId="2" r:id="rId2"/>
+    <sheet name="gl4_buoyRBRTemp.meta" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="disciplines">metadata!$T$2:$T$13</definedName>
@@ -503,6 +503,9 @@
     <t>Pieter.Johnson@colorado.edu</t>
   </si>
   <si>
+    <t>GL4.RBRTemp.data.csv</t>
+  </si>
+  <si>
     <t>30 minute timestamp data</t>
   </si>
   <si>
@@ -606,9 +609,6 @@
   </si>
   <si>
     <t xml:space="preserve">See attatched diagram for details. </t>
-  </si>
-  <si>
-    <t>gl4.buoy.RBRTemp.data.csv</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1301,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="B68" sqref="B68:I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1776,7 +1776,7 @@
         <v>51</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1860,7 +1860,7 @@
         <v>58</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2445,13 +2445,13 @@
         <v>34</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D40" s="38" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>92</v>
@@ -3036,13 +3036,13 @@
         <v>1</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C63" s="33" t="s">
         <v>119</v>
       </c>
       <c r="D63" s="33" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E63" s="29"/>
       <c r="F63" s="29"/>
@@ -3066,13 +3066,13 @@
         <v>2</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C64" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D64" s="33" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E64" s="29"/>
       <c r="F64" s="30">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="H64" s="29"/>
       <c r="I64" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -3105,7 +3105,7 @@
         <v>120</v>
       </c>
       <c r="C65" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D65" s="29" t="s">
         <v>120</v>
@@ -3136,13 +3136,13 @@
         <v>4</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D66" s="33" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E66" s="29"/>
       <c r="F66" s="40">
@@ -3153,7 +3153,7 @@
       </c>
       <c r="H66" s="29"/>
       <c r="I66" s="33" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -3172,13 +3172,13 @@
         <v>5</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D67" s="33" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E67" s="29"/>
       <c r="F67" s="29">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="H67" s="29"/>
       <c r="I67" s="33" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -23792,7 +23792,7 @@
   <dimension ref="A1:H982"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23886,7 +23886,7 @@
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -23898,7 +23898,7 @@
     </row>
     <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -23910,7 +23910,7 @@
     </row>
     <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -23922,7 +23922,7 @@
     </row>
     <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -23954,7 +23954,7 @@
     </row>
     <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -23966,7 +23966,7 @@
     </row>
     <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -23978,7 +23978,7 @@
     </row>
     <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="34" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -23990,7 +23990,7 @@
     </row>
     <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -24022,7 +24022,7 @@
     </row>
     <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -24034,7 +24034,7 @@
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -24046,7 +24046,7 @@
     </row>
     <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="34" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -24058,7 +24058,7 @@
     </row>
     <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="34" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -24070,7 +24070,7 @@
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="34" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -24082,7 +24082,7 @@
     </row>
     <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="34" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -24094,7 +24094,7 @@
     </row>
     <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="34" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -24106,7 +24106,7 @@
     </row>
     <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="34" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -24118,7 +24118,7 @@
     </row>
     <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="34" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -24152,7 +24152,7 @@
     </row>
     <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="31" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -24164,7 +24164,7 @@
     </row>
     <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="31" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -24176,7 +24176,7 @@
     </row>
     <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>

</xml_diff>